<commit_message>
progress on earth :)
</commit_message>
<xml_diff>
--- a/example/1_demo/timeline.xlsx
+++ b/example/1_demo/timeline.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3440" yWindow="2240" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="8020" yWindow="1920" windowWidth="28800" windowHeight="17600" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="initialization" sheetId="2" r:id="rId1"/>
+    <sheet name="timeline" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,17 +28,85 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="21">
   <si>
     <t>datetime</t>
+  </si>
+  <si>
+    <t>init</t>
+  </si>
+  <si>
+    <t>colony</t>
+  </si>
+  <si>
+    <t>parameter</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>structure</t>
+  </si>
+  <si>
+    <t>earth</t>
+  </si>
+  <si>
+    <t>propelant_container</t>
+  </si>
+  <si>
+    <t>booster_storage</t>
+  </si>
+  <si>
+    <t>tank_storage</t>
+  </si>
+  <si>
+    <t>heartofgold_storage</t>
+  </si>
+  <si>
+    <t>propelant_factory</t>
+  </si>
+  <si>
+    <t>booster_factory</t>
+  </si>
+  <si>
+    <t>tank_factory</t>
+  </si>
+  <si>
+    <t>heartofgold_factory</t>
+  </si>
+  <si>
+    <t>event</t>
+  </si>
+  <si>
+    <t>update</t>
+  </si>
+  <si>
+    <t>propellant_factory</t>
+  </si>
+  <si>
+    <t>rate</t>
+  </si>
+  <si>
+    <t>unit</t>
+  </si>
+  <si>
+    <t>unit/sec</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -65,8 +134,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -344,17 +415,236 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A3:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="180" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView topLeftCell="A3" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="220" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
+    <row r="3" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="220" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>45825.625</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added Mars, in progress for logging feature
</commit_message>
<xml_diff>
--- a/example/1_demo/timeline.xlsx
+++ b/example/1_demo/timeline.xlsx
@@ -9,11 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19780" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="initialization" sheetId="2" r:id="rId1"/>
-    <sheet name="timeline" sheetId="1" r:id="rId2"/>
+    <sheet name="timeline" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="21">
   <si>
     <t>datetime</t>
   </si>
@@ -69,9 +68,6 @@
     <t>event</t>
   </si>
   <si>
-    <t>update</t>
-  </si>
-  <si>
     <t>propellant_factory</t>
   </si>
   <si>
@@ -81,9 +77,6 @@
     <t>unit</t>
   </si>
   <si>
-    <t>unit/sec</t>
-  </si>
-  <si>
     <t>stock</t>
   </si>
   <si>
@@ -91,6 +84,12 @@
   </si>
   <si>
     <t>production</t>
+  </si>
+  <si>
+    <t>initial</t>
+  </si>
+  <si>
+    <t>unit/year</t>
   </si>
 </sst>
 </file>
@@ -415,258 +414,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="220" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8:D13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2">
-        <v>100</v>
-      </c>
-      <c r="E2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3">
-        <v>100</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4">
-        <v>100</v>
-      </c>
-      <c r="E4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5">
-        <v>100</v>
-      </c>
-      <c r="E5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6">
-        <v>100</v>
-      </c>
-      <c r="E6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7">
-        <v>100</v>
-      </c>
-      <c r="E7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8">
-        <v>100</v>
-      </c>
-      <c r="E8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9">
-        <v>100</v>
-      </c>
-      <c r="E9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10">
-        <v>100</v>
-      </c>
-      <c r="E10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11">
-        <v>100</v>
-      </c>
-      <c r="E11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12">
-        <v>100</v>
-      </c>
-      <c r="E12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13">
-        <v>100</v>
-      </c>
-      <c r="E13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
-  <sheetViews>
-    <sheetView zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="220" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -689,30 +446,287 @@
         <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
-        <v>45825.625</v>
+        <v>45825.5</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F2">
         <v>10</v>
       </c>
       <c r="G2" t="s">
-        <v>17</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>45825.5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3">
+        <v>6</v>
+      </c>
+      <c r="G3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>45825.5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4">
+        <v>5</v>
+      </c>
+      <c r="G4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>45825.5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>45825.5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>45825.5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7">
+        <f>365*24*60*60</f>
+        <v>31536000</v>
+      </c>
+      <c r="G7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>45825.5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8">
+        <v>6</v>
+      </c>
+      <c r="G8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>45825.5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9">
+        <f>365*24*60*60</f>
+        <v>31536000</v>
+      </c>
+      <c r="G9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>45825.5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10">
+        <v>5</v>
+      </c>
+      <c r="G10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>45825.5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11">
+        <f>365*24*60*60</f>
+        <v>31536000</v>
+      </c>
+      <c r="G11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>45825.5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
+        <v>45825.5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13">
+        <f>365*24*60*60</f>
+        <v>31536000</v>
+      </c>
+      <c r="G13" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
timeline + fix little bug
</commit_message>
<xml_diff>
--- a/example/1_demo/timeline.xlsx
+++ b/example/1_demo/timeline.xlsx
@@ -89,7 +89,7 @@
     <t>initial</t>
   </si>
   <si>
-    <t>unit/year</t>
+    <t>seconds</t>
   </si>
 </sst>
 </file>
@@ -416,8 +416,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="220" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="220" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -581,8 +581,8 @@
         <v>14</v>
       </c>
       <c r="F7">
-        <f>340*24*60*60</f>
-        <v>29376000</v>
+        <f>30*24*60*60</f>
+        <v>2592000</v>
       </c>
       <c r="G7" t="s">
         <v>20</v>
@@ -605,7 +605,7 @@
         <v>18</v>
       </c>
       <c r="F8">
-        <v>6</v>
+        <v>0.6</v>
       </c>
       <c r="G8" t="s">
         <v>15</v>
@@ -628,8 +628,8 @@
         <v>14</v>
       </c>
       <c r="F9">
-        <f>340*24*60*60</f>
-        <v>29376000</v>
+        <f>30*24*60*60</f>
+        <v>2592000</v>
       </c>
       <c r="G9" t="s">
         <v>20</v>
@@ -652,7 +652,7 @@
         <v>18</v>
       </c>
       <c r="F10">
-        <v>5</v>
+        <v>0.5</v>
       </c>
       <c r="G10" t="s">
         <v>15</v>
@@ -675,8 +675,8 @@
         <v>14</v>
       </c>
       <c r="F11">
-        <f>340*24*60*60</f>
-        <v>29376000</v>
+        <f>30*24*60*60</f>
+        <v>2592000</v>
       </c>
       <c r="G11" t="s">
         <v>20</v>
@@ -699,7 +699,7 @@
         <v>18</v>
       </c>
       <c r="F12">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="G12" t="s">
         <v>15</v>
@@ -722,8 +722,8 @@
         <v>14</v>
       </c>
       <c r="F13">
-        <f>340*24*60*60</f>
-        <v>29376000</v>
+        <f>30*24*60*60</f>
+        <v>2592000</v>
       </c>
       <c r="G13" t="s">
         <v>20</v>

</xml_diff>